<commit_message>
ModifiedHire featuresteps and offboarding files-28-09-21
</commit_message>
<xml_diff>
--- a/CucumberLearning/src/test/resources/Testdata/Data.xlsx
+++ b/CucumberLearning/src/test/resources/Testdata/Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-pborawake\git\cucumberlearningpb\CucumberLearning\src\test\resources\Testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-pborawake\git\cucumber_newlearning\CucumberLearning\src\test\resources\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F63966-FC53-401D-B270-254B57A655EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2B1C8B-C23B-4EE7-AEB9-60C88B814D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{B68B1914-19B5-45FE-87A3-165FD65F000B}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B68B1914-19B5-45FE-87A3-165FD65F000B}"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>SubjectHeading</t>
   </si>
@@ -71,15 +71,9 @@
     <t>TestSuite</t>
   </si>
   <si>
-    <t>URL</t>
-  </si>
-  <si>
     <t>StartDateType</t>
   </si>
   <si>
-    <t>StartDate</t>
-  </si>
-  <si>
     <t>Country</t>
   </si>
   <si>
@@ -95,9 +89,6 @@
     <t>PositionNo</t>
   </si>
   <si>
-    <t>RestURL</t>
-  </si>
-  <si>
     <t>ej_PositionType</t>
   </si>
   <si>
@@ -182,9 +173,6 @@
     <t>Hire</t>
   </si>
   <si>
-    <t>https://api41preview.sapsf.com/odata/v2/</t>
-  </si>
-  <si>
     <t>RP</t>
   </si>
   <si>
@@ -207,6 +195,15 @@
   </si>
   <si>
     <t>HR_Ops_CurrentWave</t>
+  </si>
+  <si>
+    <t>Enviornments</t>
+  </si>
+  <si>
+    <t>UAT</t>
+  </si>
+  <si>
+    <t>tdsstartDate</t>
   </si>
 </sst>
 </file>
@@ -294,7 +291,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -306,6 +303,7 @@
     <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -627,13 +625,13 @@
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -647,7 +645,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -661,7 +659,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -686,168 +684,172 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1BE4823-410D-4F53-B8F7-9A2E0FCF1693}">
-  <dimension ref="A1:AG2"/>
+  <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="148.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="W1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>39</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="B2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
         <v>40</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="E2" t="s">
         <v>41</v>
       </c>
-      <c r="AG1" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="F2" t="s">
         <v>42</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" t="s">
         <v>43</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>44</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>45</v>
       </c>
-      <c r="G2" t="s">
+      <c r="K2" t="s">
         <v>46</v>
       </c>
-      <c r="H2" t="s">
+      <c r="L2" t="s">
         <v>47</v>
       </c>
-      <c r="J2" t="s">
+      <c r="M2" t="s">
         <v>48</v>
       </c>
-      <c r="K2" t="s">
+      <c r="T2" t="s">
         <v>49</v>
       </c>
-      <c r="L2" t="s">
+      <c r="AD2" t="s">
         <v>50</v>
       </c>
-      <c r="M2" t="s">
-        <v>51</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="AE2">
+        <v>1</v>
+      </c>
+      <c r="AF2" t="s">
         <v>52</v>
-      </c>
-      <c r="U2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AF2">
-        <v>1</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{F8B6FF7A-C601-4670-B7B3-1F05F5E59E71}">
+      <formula1>"UAT,PREVIEW,SIT"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>